<commit_message>
Updated v1 from 1st feedback
</commit_message>
<xml_diff>
--- a/DAD5_Anaestesi_export_v1_0_0.xlsx
+++ b/DAD5_Anaestesi_export_v1_0_0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,14 +493,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>anesthesia_observation</t>
+          <t>airway_management</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Håndtering af patientens luftveje</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr">
         <is>
-          <t>OrganizationCode</t>
+          <t>MethodCode</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -510,131 +515,141 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Type af observationssted</t>
+          <t>Ekstra oplysninger til variabler: 
+- sctid41700002 = Spontan respiation
+- BGDA60 ? Maskeventilation
+- larynxmaske = Larynxmaske (alle typer)
+- kgbb00 = tracheostomi
+- andet = Ikke relevant/pt er Intuberet/tracheostomeret</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "centralt_observationsafsnit" | "andet_observationsafsnit" | "operationsgangen" | "intensiv" | "sengeafdeling" | "skadestue_modtagelse" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "sctid41700002" | "bgda60" | "larynxmaske" | "intubation" | "kgbb00" | "andet" | </t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Hvor er patienten udskrevet til?</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "stamafdeling" | "hjemmet" | "reoperation" | "intensiv_afdeling" | "andet_hospital" | "doed_i_observationsperioden" | </t>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>airway_management_last_attempt</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sidste forsøg på håndtering af patientens luftveje
+lma = alle typer</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="D5" t="inlineStr">
         <is>
-          <t>DateTimeEnd</t>
+          <t>MethodCode</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ekstra oplysninger til udfald:
+- sctid257268009 = LMA (alle typer)
+- sctid78121007 = Direkte laryngoskopi
+- kgba00a  = Nødtracheostomi
+</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t xml:space="preserve">Enums/Udfald: | "sctid257268009" | "sctid78121007" | "videolaryngoskopi" | "fleksibelt_skopi" | "vaekning_af_patient" | "kgba00a" | "anden_teknik" | </t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>DateTimeStart</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SOR_anesthesia</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SOR-koden for anæstesiafdelingen</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>OrganizationCode</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Activity</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>relaxation_intubation</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Relaksation til intubation</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>anesthesia_observation</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>OrganizationCode</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>str, Enum</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Kun relevant hvis Luftvejshåndtering = Intubation</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "nej" | "depolariserende" | "non_depolariserende" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>airway_management</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Håndtering af patientens luftveje</t>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Type af observationssted (opvågningssted)</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "centralt_observationsafsnit" | "andet_observationsafsnit" | "operationsgangen" | "intensiv" | "sengeafdeling" | "skadestue_modtagelse" | </t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="D10" t="inlineStr">
         <is>
-          <t>MethodCode</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -642,31 +657,40 @@
           <t>str, Enum</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hvor er patienten udskrevet til?
+Ekstra oplysninger til udfald: 
+- sctid261554009 = Reoperation
+- sctid310032008 = Intensiv afdeling
+</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "kun_spontan_respiration" | "maskeventilation" | "larynxmaske" | "intubation" | "tracheostomi" | "ikke_relevant" | "intuberet" | "tracheostomeret" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "stamafdeling" | "hjemmet" | "sctid261554009" | "sctid310032008" | "andet_hospital" | "doed_i_observationsperioden" | </t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>service_time</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Start og slut ydelse</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>True</t>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>DateTimeEnd</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Sluttidspunkt (datotid) for opvågning</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
     </row>
@@ -683,7 +707,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Start tidspunkt for anæstesi-ydelse</t>
+          <t>Starttidspunkt (datotid) for opvågning</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -691,53 +715,48 @@
           <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Activity</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>service_time</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Start og slut ydelse</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>True</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="D13" t="inlineStr">
+    <row r="14">
+      <c r="D14" t="inlineStr">
         <is>
           <t>DateTimeEnd</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>str</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>Sluttidspunkt for anæstesi-ydelse</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Activity</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>procedure_code</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>SKS-kode for den **vigtigste ** procedure foretaget under anæstesien</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -749,12 +768,22 @@
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>DateTimeStart</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>String</t>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Start tidspunkt for anæstesi-ydelse</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -771,19 +800,24 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SOR_code</t>
+          <t>procedure_code</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>SOR-koden for anæstesiafdelingen</t>
+          <t>SKS-kode for den **vigtigste ** procedure foretaget under anæstesien</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="D17" t="inlineStr">
         <is>
-          <t>OrganizationCode</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -805,20 +839,19 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>airway_management_last_attempt</t>
+          <t>intubation</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Sidste forsøg på håndtering af patientens luftveje
-lma = alle typer</t>
+          <t>Typen af intubation</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="D19" t="inlineStr">
         <is>
-          <t>MethodCode</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -826,9 +859,20 @@
           <t>str, Enum</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>*Kun relevant hvis Luftvejshåndtering == Intubation*
+Ekstra oplysninger til udfald: 
+- laryngoskopi_max2 = Højest 2 forsøg, seneste ved direkte laryngoskopi
+- videolaryngoskopi_max2 = Højest 2 forsøg, seneste ved videolaryngoskopi
+- fleksibel_skopi_max2 = Højest 2 forsøg, seneste ved fleksibel skopi
+- andet_max2 = Højest 2 forsøg seneste ved andet end ovennævnte metoder
+- mere_end_3 = 3 forsøg eller flere uanset metode</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "lma" | "direkte_laryngoskopi" | "videolaryngoskopi" | "fleksibelt_skopi" | "vaekning_af_patient" | "noedtracheostomi" | "anden_teknik" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "laryngoskopi_max2" | "videolaryngoskopi_max2" | "fleksibel_skopi_max2" | "andet_max2" | "mere_end_3" | "intubation_opgivet" | </t>
         </is>
       </c>
     </row>
@@ -840,19 +884,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>intubation</t>
+          <t>airaway_plan</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Typen af intubation</t>
+          <t>Plan for håndteringen af patientens luftveje</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="D21" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>MethodCode</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -862,12 +906,21 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Kun relevant hvis Luftvejshåndtering == Intubation</t>
+          <t xml:space="preserve">- sctid241700002 = Spontan_respiration
+- bgda60 = Maskeventilation
+- sctid257268009 = Larynxmaske(alle typer)
+- intubation_laryngoskopi = Intubation ved direkte laryngoskopi
+- intubation_videolaryngoskopi = Intubation med videolaryngoskopi
+- intubation_fleksibelt_skop = Intubation med fleksibelt skop
+- intubation_anden_metode = Intubation ved anden metode
+- tracheostomi_lokalanæstesi = Tracheostomi i lokalanæstesi
+- intuberet_tracheostomeret = Er intuberet/tracheostomeret
+</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "laryngoskopi_max2" | "videolaryngoskopi_max2" | "fleksibel_skopi_max2" | "andet_max2" | "mere_end_3" | "intubation_opgivet" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "sctid241700002" | "bgda60" | "sctid257268009" | "intubation_laryngoskopi" | "intubation_videolaryngoskopi" | "intubation_anden_metode" | "tracheostomi_lokalanaestesi" | "intuberet_tracheostomeret" | </t>
         </is>
       </c>
     </row>
@@ -879,19 +932,19 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>airaway_plan</t>
+          <t>relaxation_intubation</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Plan for håndteringen af patientens luftveje</t>
+          <t>Relaksation til intubation</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="D23" t="inlineStr">
         <is>
-          <t>MethodCode</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -899,9 +952,18 @@
           <t>str, Enum</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Kun relevant hvis Luftvejshåndtering = Intubation
+Ekstra oplysninger til udfald:
+- vv00003  = nej
+- sctid22587006 = Depolariserende
+- sctid59594008 = Non-depolariserende</t>
+        </is>
+      </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "spontan_respiration" | "maskeventilation" | "larynxmaske_alle_typer" | "intubation_direkte_laryngoskopi" | "intubation_videolaryngoskopi" | "intubation_anden_metode" | "tracheostomi_lokalanaestesi" | "intuberet_tracheostomeret" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "vv00003" | "sctid22587006" | "sctid59594008" | </t>
         </is>
       </c>
     </row>
@@ -933,9 +995,18 @@
           <t>str, Enum</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Ekstra oplysninger til udfald:
+- sctid72641008 = Sedation
+- sctid225419007 = Overvågning
+- NAAC3 =  IV og inhalation
+- NAAC1 = TIVA</t>
+        </is>
+      </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "perifer_nerveblokade" | "central_blokade" | "sedation" | "overvaagning" | "inhalation" | "iv_inhalation" | "tiva" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "perifer_nerveblokade" | "central_blokade" | "sctid72641008" | "sctid225419007" | "inhalation" | "naac3" | "naac1" | </t>
         </is>
       </c>
     </row>
@@ -947,29 +1018,38 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ASA_score</t>
+          <t>pain_on_arrival</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Patientens ASA-score</t>
+          <t>Smerte-score (NRS eller FLACC) mindre end 15 minutter efter ankomst til observationsstedet</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="D27" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smerte-score (NRS eller FLACC) mindre end 15 minutter efter ankomst til opvågningen
+*Kun relevant hvis Observationssted = Centralt observationsafsnit
+ELLER
+Observationssted = Andet observationsafsnit*
+</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "asa_i" | "asa_ii" | "asa_iii" | "asa_iv" | "asa_v" | "asa_vi" | </t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 10</t>
         </is>
       </c>
     </row>
@@ -981,400 +1061,27 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>pain_on_arrival</t>
+          <t>best_achieved_laryngoscopy_grade</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Smerte-score (NRS eller FLACC) mindre end 15 minutter efter ankomst til observationsstedet</t>
+          <t>Bedst opnåede laryngoskopigrad</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="D29" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
-        <is>
-          <t>Kun relevant hvis Observationssted = Centralt observationsafsnit
-ELLER
-Observationssted = Andet observationsafsnit</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>nausea_on_arrival</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Kvalme-score mindre end 15 minutter efter ankomst til observationsstedet</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Kun relevant hvis Observationssted = Centralt observationsafsnit
-ELLER
-Observationssted = Andet observationsafsnit</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>blockade_sufficiency</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Virkede blokaden sufficient?</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>anesthesia_prioritization</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Hvor akut var anæstesien?</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "elektiv" | "fremskyndet" | "hastende" | "umiddelbart_livstruende" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>pain_at_discharge</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Smerte-score (NRS eller FLACC)  mindre end 15 minutter før udskrivelse og transport fra observationsstedet</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Kun relevant hvis Observationssted = Centralt observationsafsnit
-ELLER
-Observationssted = Andet observationsafsnit</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 10</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>anesthesia_no_complications</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Har anæstesien været uden komplikationer?</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>anesthesia_complications</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Komplikationer opstået under anæstesien</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Kun relevant hvis komplikationer = Nej</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "anafylaktisk_reaktion_shock" | "_anaestesi_afbrudt" | "aspiration" | "durapunktur_accidentel" | "hjertestop" | "huskeanaestesi" | "malign_hypertermi_mistanke" | "neuromuskulaer_blokade_forlaenget_virkning" | "tandskade" | "mors_uventet" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>observation_complications</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Komplikationer opstået under observationen</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Kun relevant hvis Observation ingen komplikationer = Nej</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "anafylaktisk_reaktion_shock" | "aspiration" | "durapunktur_accidentel" | "hjertestop" | "huskeanaestesi" | "neuromuskulaer_blokade_forlaenget_virkning" | "tandskade" | "mors_uventet" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>observation_no_complications</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Har observationen været uden komplikationer?</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Kun relevant hvis Observationssted = Centralt observationsafsnit
-ELLER
-Observationssted = Andet observationsafsnit</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "ja" | "nej" | </t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>temperature</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Hvilken temperatur har patienten ved anæstesiens afslutning</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Integer</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>best_achieved_laryngoscopy_grade</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Bedst opnåede laryngoskopigrad</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>ResultCode</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>str, Enum</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
         <is>
           <t>Kun relevant hvis Intubation = 3 forsøg eller flere uanset metode
 Intubation opgivet
@@ -1382,50 +1089,371 @@
 Intubation=Intubation opgivet</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t xml:space="preserve">Enums/Udfald: | "grad_1" | "grad_2" | "grad_3" | "grad_4" | </t>
         </is>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+    <row r="30">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>temperature</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Hvilken temperatur har patienten ved anæstesiens afslutning</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Float</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>observation_complications</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Komplikationer opstået under observationen</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>ResultCode</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Komplikationer opstået under opvågningen
+Ekstra oplysninger til udfald:
+- di46 = Hjertestop
+- dt884a = Tandskade
+*Kun relevant hvis Observation ingen komplikationer = Nej*
+</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "anafylaktisk_reaktion_shock" | "aspiration" | "durapunktur_accidentel" | "di46" | "huskeanaestesi" | "neuromuskulaer_blokade_forlaenget_virkning" | "dt884a" | "mors_uventet" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>nausea_on_arrival</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Kvalme-score mindre end 15 minutter efter ankomst til observationsstedet</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Kvalme-score mindre end 15 minutter efter ankomst til opvågningen
+*Kun relevant hvis Observationssted = Centralt observationsafsnit
+ELLER
+Observationssted = Andet observationsafsnit*</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>ASA_score</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Patientens ASA-score</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>ResultCode</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "asa_i" | "asa_ii" | "asa_iii" | "asa_iv" | "asa_v" | "asa_vi" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>anesthesia_complications</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Komplikationer opstået under anæstesien</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>ResultCode</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*Kun relevant hvis komplikationer = Nej*
+Ekstra oplysninger til udfald:
+- di46 = Hjertestop
+- dt883 = Malign Hypertermi mistanke
+- dt884a = Tandskade
+</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "anafylaktisk_reaktion_shock" | "_anaestesi_afbrudt" | "aspiration" | "durapunktur_accidentel" | "di46" | "huskeanaestesi" | "dt883" | "neuromuskulaer_blokade_forlaenget_virkning" | "dt884a" | "mors_uventet" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>pain_at_discharge</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Smerte-score (NRS eller FLACC)  mindre end 15 minutter før udskrivelse og transport fra observationsstedet</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Smerte-score (NRS eller FLACC)  mindre end 15 minutter før udskrivelse og transport fra opvågningen
+*Kun relevant hvis Observationssted = Centralt observationsafsnit
+ELLER
+Observationssted = Andet observationsafsnit*
+</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0 | Less than or equal to: 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>nausea_at_discharge</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>Kvalme-score mindre end 15 minutter før udskrivelse og transport fra observationsstedet</t>
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="D51" t="inlineStr">
+    <row r="43">
+      <c r="D43" t="inlineStr">
         <is>
           <t>ResultValue</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>Integer</t>
         </is>
       </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Kun relevant hvis Observationssted = Centralt observationsafsnit
+      <c r="F43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kvalme-score mindre end 15 minutter før udskrivelse og transport fra opvågningen 
+*Kun relevant hvis Observationssted = Centralt observationsafsnit
 ELLER
-Observationssted = Andet observationsafsnit</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
+Observationssted = Andet observationsafsnit*
+</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
         <is>
           <t>Greater than or equal to: 0 | Less than or equal to: 10</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>blockade_sufficiency</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Virkede blokaden sufficient?</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>ResultCode</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Ekstra oplysninger til udfald: 
+- vv00002 = ja
+- vv00003  = nej</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "vv00002" | "vv00003" | </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>anesthesia_prioritization</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Hvor akut var anæstesien?</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>ResultCode</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>- sctid103390000 = Elektiv
+- fremskyndet  = Fremskyndet (dage)
+- hastende = Hastende (timer)
+- livstruende = Umiddelbart livstruende</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Enums/Udfald: | "sctid103390000" | "fremskyndet" | "hastende" | "livstruende" | </t>
         </is>
       </c>
     </row>

</xml_diff>